<commit_message>
Restructure code, use dockable UI, add About dialog, fix bugs, add another input
</commit_message>
<xml_diff>
--- a/NutrientTargetData.xlsx
+++ b/NutrientTargetData.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="205">
   <si>
     <t>g</t>
   </si>
@@ -778,10 +778,13 @@
     <t>Target is "as low as possible" but https://www.healthline.com/nutrition/dietary-cholesterol-does-not-matter suggests it's unimportant</t>
   </si>
   <si>
-    <t>This is total vitamin A in retinol equivalent units</t>
-  </si>
-  <si>
     <t>(listed in milligrams in the table I used. Also, tap water may have around 600-700 micrograms per liter, so over half of the daily value if you drink the recommended amount of water)</t>
+  </si>
+  <si>
+    <t>This is total vitamin A in retinol equivalent units, but it's not always used, unlike the IU measure</t>
+  </si>
+  <si>
+    <t>3.33 IU = 1 microgram RAE in some cases, or 20 IU = 1 microgram RAE in others--see the sr28_doc</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2107,7 +2112,7 @@
         <v>30</v>
       </c>
       <c r="M29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -2200,7 +2205,9 @@
       <c r="L32" t="s">
         <v>34</v>
       </c>
-      <c r="M32" s="3"/>
+      <c r="M32" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33">
@@ -2248,11 +2255,11 @@
         <v>3000</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F34" si="2">IF(D34=0,100,100/D34)</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G34" si="3">IF(E34=D34,100,100/(E34-D34))</f>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="K34" s="1" t="s">
@@ -2262,7 +2269,7 @@
         <v>30</v>
       </c>
       <c r="M34" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -3286,11 +3293,11 @@
         <v>1</v>
       </c>
       <c r="F68" s="5">
-        <f t="shared" ref="F68:F113" si="2">IF(D68=0,100,100/D68)</f>
+        <f t="shared" ref="F68:F113" si="4">IF(D68=0,100,100/D68)</f>
         <v>370.37037037037032</v>
       </c>
       <c r="G68" s="5">
-        <f t="shared" ref="G68:G79" si="3">IF(E68=D68,100,100/(E68-D68))</f>
+        <f t="shared" ref="G68:G79" si="5">IF(E68=D68,100,100/(E68-D68))</f>
         <v>136.98630136986301</v>
       </c>
       <c r="K68" s="1" t="s">
@@ -3317,11 +3324,11 @@
         <v>3</v>
       </c>
       <c r="F69" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>185.52875695732837</v>
       </c>
       <c r="G69" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40.633888663145065</v>
       </c>
       <c r="K69" s="1" t="s">
@@ -3348,11 +3355,11 @@
         <v>5</v>
       </c>
       <c r="F70" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>129.87012987012986</v>
       </c>
       <c r="G70" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23.640661938534276</v>
       </c>
       <c r="K70" s="1" t="s">
@@ -3382,11 +3389,11 @@
         <v>5</v>
       </c>
       <c r="F71" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>92.764378478664185</v>
       </c>
       <c r="G71" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25.497195308516066</v>
       </c>
       <c r="K71" s="1" t="s">
@@ -3413,11 +3420,11 @@
         <v>5</v>
       </c>
       <c r="F72" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>108.22510822510822</v>
       </c>
       <c r="G72" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>24.533856722276745</v>
       </c>
       <c r="K72" s="1" t="s">
@@ -3444,11 +3451,11 @@
         <v>5</v>
       </c>
       <c r="F73" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>99.900099900099917</v>
       </c>
       <c r="G73" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25.006251562890721</v>
       </c>
       <c r="K73" s="1" t="s">
@@ -3507,11 +3514,11 @@
         <v>5</v>
       </c>
       <c r="F75" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>92.764378478664185</v>
       </c>
       <c r="G75" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25.497195308516066</v>
       </c>
       <c r="K75" s="1" t="s">
@@ -3570,11 +3577,11 @@
         <v>5</v>
       </c>
       <c r="F77" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>129.87012987012986</v>
       </c>
       <c r="G77" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23.640661938534276</v>
       </c>
       <c r="K77" s="1" t="s">
@@ -3630,11 +3637,11 @@
         <v>5</v>
       </c>
       <c r="F79" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>129.87012987012986</v>
       </c>
       <c r="G79" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23.640661938534276</v>
       </c>
       <c r="K79" s="1" t="s">
@@ -4395,7 +4402,7 @@
         <v>99999</v>
       </c>
       <c r="F105" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>333.33333333333337</v>
       </c>
       <c r="G105" s="5">
@@ -4573,7 +4580,7 @@
         <v>99999</v>
       </c>
       <c r="F111" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>555.55555555555554</v>
       </c>
       <c r="G111" s="5">
@@ -4635,7 +4642,7 @@
         <v>99999</v>
       </c>
       <c r="F113" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>769.23076923076917</v>
       </c>
       <c r="G113" s="5">
@@ -5527,11 +5534,11 @@
         <v>99999</v>
       </c>
       <c r="F143" s="5">
-        <f t="shared" ref="F143" si="4">IF(D143=0,100,100/D143)</f>
+        <f t="shared" ref="F143" si="6">IF(D143=0,100,100/D143)</f>
         <v>76.92307692307692</v>
       </c>
       <c r="G143" s="5">
-        <f t="shared" ref="G143" si="5">IF(E143=D143,100,100/(E143-D143))</f>
+        <f t="shared" ref="G143" si="7">IF(E143=D143,100,100/(E143-D143))</f>
         <v>1.0000230005290122E-3</v>
       </c>
       <c r="K143" s="1" t="s">

</xml_diff>